<commit_message>
grap clip step 추가
</commit_message>
<xml_diff>
--- a/Data/Test/dataset17/input_data.xlsx
+++ b/Data/Test/dataset17/input_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sueng\PycharmProjects\AI_SH_graph_rev_rev1\Data\Test\dataset17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sueng\PycharmProjects\experiment\AI_SH_graph_rev_rev1\Data\Test\dataset17\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D43FD4-7377-4A41-B86B-D18EDCF26167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A610FB-DF03-412B-BC32-CC0EEDAC7262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4920" yWindow="4875" windowWidth="17370" windowHeight="7680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ship" sheetId="1" r:id="rId1"/>
@@ -571,17 +571,17 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="5" width="8.796875" style="1"/>
-    <col min="6" max="7" width="8.796875" style="2"/>
-    <col min="8" max="9" width="8.796875" style="3"/>
+    <col min="4" max="5" width="8.75" style="1"/>
+    <col min="6" max="7" width="8.75" style="2"/>
+    <col min="8" max="9" width="8.75" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -610,7 +610,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -639,7 +639,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -668,7 +668,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -697,7 +697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -726,7 +726,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -755,7 +755,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -784,7 +784,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -813,7 +813,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -842,7 +842,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -871,7 +871,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -900,7 +900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -929,7 +929,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -958,7 +958,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -987,7 +987,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>6000000</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>9300</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1699,9 +1699,9 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1771,7 +1771,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>9300</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -1939,9 +1939,9 @@
       <selection sqref="A1:E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>9300</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -2227,9 +2227,9 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -2320,9 +2320,9 @@
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>60</v>
       </c>

</xml_diff>